<commit_message>
Default duration of class is ero
</commit_message>
<xml_diff>
--- a/computed_grades.xlsx
+++ b/computed_grades.xlsx
@@ -475,10 +475,10 @@
         <v>1</v>
       </c>
       <c r="C2">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D2">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:4">
@@ -489,7 +489,7 @@
         <v>2</v>
       </c>
       <c r="C3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D3">
         <v>0</v>
@@ -506,7 +506,7 @@
         <v>0</v>
       </c>
       <c r="D4">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>